<commit_message>
Added more notes about software used in this project and added the .NET platform
</commit_message>
<xml_diff>
--- a/docs/software_bom.xlsx
+++ b/docs/software_bom.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27030"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakmad\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF8FE00-00E7-4597-A898-3AA1A7BAF4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9B3BEC6-0A0E-49DF-84E7-D8A2C1AFAE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -28,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Component Name</t>
   </si>
@@ -51,15 +65,90 @@
     <t>Dependency Type</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>Unity3D</t>
   </si>
   <si>
+    <t>Unity Technologies</t>
+  </si>
+  <si>
     <t>2022.3.5f1</t>
   </si>
   <si>
+    <t>Proprietary</t>
+  </si>
+  <si>
+    <t>Subscription</t>
+  </si>
+  <si>
+    <t>Development/Runtime</t>
+  </si>
+  <si>
+    <t>Used for developing simulation - this software is used both as a tool and as a core component of the software used in the project</t>
+  </si>
+  <si>
+    <t>.NET Platform</t>
+  </si>
+  <si>
+    <t>Microsoft and Unity Technologies</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>Perpetual</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Used by Unity for the runtime - this software is used as a core component of the software developed in this project</t>
+  </si>
+  <si>
+    <t>Blender</t>
+  </si>
+  <si>
+    <t>Blender Foundation</t>
+  </si>
+  <si>
+    <t>3.6.5</t>
+  </si>
+  <si>
+    <t>GPL-2.0-or-later</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Used for creating assets - this software is used as a tool, not as part of the software developed in this project</t>
+  </si>
+  <si>
+    <t>GIMP</t>
+  </si>
+  <si>
+    <t>GIMP Development Team</t>
+  </si>
+  <si>
+    <t>2.10.34</t>
+  </si>
+  <si>
+    <t>GPL-3.0-or-later</t>
+  </si>
+  <si>
     <t>VSCode</t>
   </si>
   <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
     <t>1.83.1</t>
   </si>
   <si>
@@ -69,112 +158,58 @@
     <t>MS-PL</t>
   </si>
   <si>
-    <t>Development</t>
-  </si>
-  <si>
-    <t>Subscription</t>
-  </si>
-  <si>
-    <t>Perpetual</t>
-  </si>
-  <si>
-    <t>Development/Deployment</t>
+    <t>Used for developing simulation - this software is used as a tool, not as part of the software developed in this project</t>
+  </si>
+  <si>
+    <t>Amazon Web Services</t>
+  </si>
+  <si>
+    <t>ADSL</t>
   </si>
   <si>
     <t>Deployment</t>
   </si>
   <si>
+    <t>Used for hosting - this software is used as a tool, not as part of the software developed in this project</t>
+  </si>
+  <si>
+    <t>Ubuntu Server</t>
+  </si>
+  <si>
+    <t>Canonical</t>
+  </si>
+  <si>
+    <t>22.04.3</t>
+  </si>
+  <si>
+    <t>GPL-1.0-or-later</t>
+  </si>
+  <si>
+    <t>Used for serving website - this software is used as a tool, not as part of the software developed in this project</t>
+  </si>
+  <si>
+    <t>Apache HTTP Server</t>
+  </si>
+  <si>
+    <t>Apache Software Foundation</t>
+  </si>
+  <si>
+    <t>2.4.58</t>
+  </si>
+  <si>
+    <t>Apache-2.0</t>
+  </si>
+  <si>
+    <t>MariaDB</t>
+  </si>
+  <si>
+    <t>MariaDB Foundation</t>
+  </si>
+  <si>
     <t>PHP</t>
   </si>
   <si>
-    <t>MariaDB</t>
-  </si>
-  <si>
-    <t>Ubuntu Server</t>
-  </si>
-  <si>
-    <t>22.04.3</t>
-  </si>
-  <si>
-    <t>Apache HTTP Server</t>
-  </si>
-  <si>
-    <t>GPL-1.0-or-later</t>
-  </si>
-  <si>
-    <t>Amazon Web Services</t>
-  </si>
-  <si>
-    <t>ADSL</t>
-  </si>
-  <si>
-    <t>Blender</t>
-  </si>
-  <si>
-    <t>Proprietary</t>
-  </si>
-  <si>
-    <t>GPL-2.0-or-later</t>
-  </si>
-  <si>
-    <t>3.6.5</t>
-  </si>
-  <si>
-    <t>GIMP</t>
-  </si>
-  <si>
-    <t>GPL-3.0-or-later</t>
-  </si>
-  <si>
-    <t>2.10.34</t>
-  </si>
-  <si>
-    <t>2.4.58</t>
-  </si>
-  <si>
-    <t>Apache-2.0</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Used for developing simulation</t>
-  </si>
-  <si>
-    <t>Used for creating assets</t>
-  </si>
-  <si>
-    <t>Used for hosting</t>
-  </si>
-  <si>
-    <t>Used for serving website</t>
-  </si>
-  <si>
-    <t>Unity Technologies (https://unity.com/)</t>
-  </si>
-  <si>
-    <t>Blender Foundation (https://www.blender.org/)</t>
-  </si>
-  <si>
-    <t>GIMP Development Team (https://www.gimp.org/)</t>
-  </si>
-  <si>
-    <t>Microsoft (https://code.visualstudio.com/)</t>
-  </si>
-  <si>
-    <t>Amazon Web Services (https://aws.amazon.com/)</t>
-  </si>
-  <si>
-    <t>Canonical (https://ubuntu.com/)</t>
-  </si>
-  <si>
-    <t>Apache Software Foundation (https://httpd.apache.org/)</t>
-  </si>
-  <si>
-    <t>MariaDB Foundation (https://mariadb.org/)</t>
-  </si>
-  <si>
-    <t>PHP Development Team (https://www.php.net/)</t>
+    <t>PHP Development Team</t>
   </si>
 </sst>
 </file>
@@ -191,11 +226,10 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial Unicode MS"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,11 +255,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,20 +572,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -563,10 +598,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -579,245 +614,271 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4">
         <v>2025</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2025</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>37</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4">
         <v>2025</v>
       </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2025</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2027</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2027</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2025</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2025</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" s="4">
-        <v>10.11</v>
-      </c>
-      <c r="D9" s="4">
-        <v>2028</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C10" s="4">
+        <v>10.11</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2028</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="4">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D11" s="4">
         <v>2024</v>
       </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>39</v>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H10" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
@@ -825,4 +886,169 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007728E26C6A27DF4DB3EEBD400E02F0F7" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9863e01137b4adf82fec53a47779d702">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="082371fa-5688-4994-8677-8e53978ae0be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a9ab35ebebe36efe4f9f4a09220b172" ns2:_="">
+    <xsd:import namespace="082371fa-5688-4994-8677-8e53978ae0be"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="082371fa-5688-4994-8677-8e53978ae0be" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0D7379-7927-4ECB-9198-0395C1F7D689}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78F97FC-225C-4EFC-AE0E-AB171BAA814C}"/>
 </file>
</xml_diff>

<commit_message>
Added Unity models/assets to software BOM list
</commit_message>
<xml_diff>
--- a/docs/software_bom.xlsx
+++ b/docs/software_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakmad\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9B3BEC6-0A0E-49DF-84E7-D8A2C1AFAE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB4C09F-74B5-46A7-9381-0103F2C4D1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>Component Name</t>
   </si>
@@ -210,13 +210,28 @@
   </si>
   <si>
     <t>PHP Development Team</t>
+  </si>
+  <si>
+    <t>SimplePoly City</t>
+  </si>
+  <si>
+    <t>VenCreations</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>Extension Asset</t>
+  </si>
+  <si>
+    <t>Used for developing models for the simulation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -572,13 +587,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -591,7 +606,7 @@
     <col min="9" max="16384" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -643,7 +658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -669,7 +684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -695,7 +710,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -721,7 +736,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -747,7 +762,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -773,7 +788,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
@@ -799,7 +814,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>48</v>
       </c>
@@ -825,7 +840,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>52</v>
       </c>
@@ -851,7 +866,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>54</v>
       </c>
@@ -875,6 +890,32 @@
       </c>
       <c r="H11" s="3" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -889,15 +930,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007728E26C6A27DF4DB3EEBD400E02F0F7" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9863e01137b4adf82fec53a47779d702">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="082371fa-5688-4994-8677-8e53978ae0be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a9ab35ebebe36efe4f9f4a09220b172" ns2:_="">
     <xsd:import namespace="082371fa-5688-4994-8677-8e53978ae0be"/>
@@ -1035,6 +1067,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1042,13 +1083,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0D7379-7927-4ECB-9198-0395C1F7D689}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="082371fa-5688-4994-8677-8e53978ae0be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0D7379-7927-4ECB-9198-0395C1F7D689}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78F97FC-225C-4EFC-AE0E-AB171BAA814C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78F97FC-225C-4EFC-AE0E-AB171BAA814C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated software BOM to reflect currently used version of Unity
</commit_message>
<xml_diff>
--- a/docs/software_bom.xlsx
+++ b/docs/software_bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakmad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakmad\Documents\ltn-demonstrator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB4C09F-74B5-46A7-9381-0103F2C4D1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ED9235-3EA2-4FD4-B3D4-D7EC0E44E6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Unity Technologies</t>
   </si>
   <si>
-    <t>2022.3.5f1</t>
-  </si>
-  <si>
     <t>Proprietary</t>
   </si>
   <si>
@@ -225,6 +222,9 @@
   </si>
   <si>
     <t>Used for developing models for the simulation</t>
+  </si>
+  <si>
+    <t>2022.3.13f1</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -640,212 +640,212 @@
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4">
         <v>2025</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="4">
         <v>2025</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="D5" s="4">
         <v>2025</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="D8" s="4">
         <v>2027</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D9" s="4">
         <v>2025</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C10" s="4">
         <v>10.11</v>
@@ -854,24 +854,24 @@
         <v>2028</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C11" s="4">
         <v>8.1999999999999993</v>
@@ -880,42 +880,42 @@
         <v>2024</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -930,6 +930,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007728E26C6A27DF4DB3EEBD400E02F0F7" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9863e01137b4adf82fec53a47779d702">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="082371fa-5688-4994-8677-8e53978ae0be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a9ab35ebebe36efe4f9f4a09220b172" ns2:_="">
     <xsd:import namespace="082371fa-5688-4994-8677-8e53978ae0be"/>
@@ -1067,15 +1076,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1083,6 +1083,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0D7379-7927-4ECB-9198-0395C1F7D689}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1100,14 +1108,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78F97FC-225C-4EFC-AE0E-AB171BAA814C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated software BOM to remove extra software
</commit_message>
<xml_diff>
--- a/docs/software_bom.xlsx
+++ b/docs/software_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakmad\Documents\ltn-demonstrator\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Ahmad\University\ECMM427\ltn-demonstrator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ED9235-3EA2-4FD4-B3D4-D7EC0E44E6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B818A9-9E15-46D4-8DF8-1C627EE24525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Component Name</t>
   </si>
@@ -156,57 +156,6 @@
   </si>
   <si>
     <t>Used for developing simulation - this software is used as a tool, not as part of the software developed in this project</t>
-  </si>
-  <si>
-    <t>Amazon Web Services</t>
-  </si>
-  <si>
-    <t>ADSL</t>
-  </si>
-  <si>
-    <t>Deployment</t>
-  </si>
-  <si>
-    <t>Used for hosting - this software is used as a tool, not as part of the software developed in this project</t>
-  </si>
-  <si>
-    <t>Ubuntu Server</t>
-  </si>
-  <si>
-    <t>Canonical</t>
-  </si>
-  <si>
-    <t>22.04.3</t>
-  </si>
-  <si>
-    <t>GPL-1.0-or-later</t>
-  </si>
-  <si>
-    <t>Used for serving website - this software is used as a tool, not as part of the software developed in this project</t>
-  </si>
-  <si>
-    <t>Apache HTTP Server</t>
-  </si>
-  <si>
-    <t>Apache Software Foundation</t>
-  </si>
-  <si>
-    <t>2.4.58</t>
-  </si>
-  <si>
-    <t>Apache-2.0</t>
-  </si>
-  <si>
-    <t>MariaDB</t>
-  </si>
-  <si>
-    <t>MariaDB Foundation</t>
-  </si>
-  <si>
-    <t>PHP</t>
-  </si>
-  <si>
-    <t>PHP Development Team</t>
   </si>
   <si>
     <t>SimplePoly City</t>
@@ -587,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -640,7 +589,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4">
         <v>2025</v>
@@ -767,155 +716,25 @@
         <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2027</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="4">
-        <v>2025</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="4">
-        <v>10.11</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2028</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2024</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -930,15 +749,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007728E26C6A27DF4DB3EEBD400E02F0F7" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9863e01137b4adf82fec53a47779d702">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="082371fa-5688-4994-8677-8e53978ae0be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a9ab35ebebe36efe4f9f4a09220b172" ns2:_="">
     <xsd:import namespace="082371fa-5688-4994-8677-8e53978ae0be"/>
@@ -1076,6 +886,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1083,14 +902,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0D7379-7927-4ECB-9198-0395C1F7D689}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1108,6 +919,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78F97FC-225C-4EFC-AE0E-AB171BAA814C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added Git to software bill of materials
</commit_message>
<xml_diff>
--- a/docs/software_bom.xlsx
+++ b/docs/software_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Ahmad\University\ECMM427\ltn-demonstrator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B818A9-9E15-46D4-8DF8-1C627EE24525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44F5B10-C2E4-4FC1-BABB-183F38E8EC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Component Name</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>2022.3.13f1</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Git Development Team</t>
+  </si>
+  <si>
+    <t>2.44.0</t>
+  </si>
+  <si>
+    <t>Used for source control management</t>
   </si>
 </sst>
 </file>
@@ -240,9 +252,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -280,7 +292,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -386,7 +398,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -528,7 +540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -536,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -737,6 +749,32 @@
         <v>42</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -749,6 +787,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007728E26C6A27DF4DB3EEBD400E02F0F7" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9863e01137b4adf82fec53a47779d702">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="082371fa-5688-4994-8677-8e53978ae0be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a9ab35ebebe36efe4f9f4a09220b172" ns2:_="">
     <xsd:import namespace="082371fa-5688-4994-8677-8e53978ae0be"/>
@@ -886,15 +933,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -902,6 +940,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0D7379-7927-4ECB-9198-0395C1F7D689}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -919,14 +965,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF846C-E945-4042-974C-E2D5391516AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78F97FC-225C-4EFC-AE0E-AB171BAA814C}">
   <ds:schemaRefs>

</xml_diff>